<commit_message>
Init projet SSIS, SQL
</commit_message>
<xml_diff>
--- a/01 - Documentations/01 - Sources de données/Contrat_Interface_V0.01_01092017.xlsx
+++ b/01 - Documentations/01 - Sources de données/Contrat_Interface_V0.01_01092017.xlsx
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="Référence" sheetId="1" r:id="rId1"/>
     <sheet name="Carractéristiques_établissement" sheetId="2" r:id="rId2"/>
+    <sheet name="Employabilité" sheetId="3" r:id="rId3"/>
+    <sheet name="Référentiel" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t xml:space="preserve">Référence du document </t>
   </si>
@@ -133,6 +135,165 @@
   </si>
   <si>
     <t>ID_CarracteristiqueEtablissement</t>
+  </si>
+  <si>
+    <t>BL_IsActif</t>
+  </si>
+  <si>
+    <t>ID_StatutActivite</t>
+  </si>
+  <si>
+    <t>ID_TrancheAge</t>
+  </si>
+  <si>
+    <t>BL_IsAideFamilial</t>
+  </si>
+  <si>
+    <t>DT_Year</t>
+  </si>
+  <si>
+    <t>ID_TypeEntreprise</t>
+  </si>
+  <si>
+    <t>ID_Contrat</t>
+  </si>
+  <si>
+    <t>BL_IsMarie</t>
+  </si>
+  <si>
+    <t>ID_CauseNouveauEmploi</t>
+  </si>
+  <si>
+    <t>ID_CategorieSociopro</t>
+  </si>
+  <si>
+    <t>ID_Diplôme</t>
+  </si>
+  <si>
+    <t>ID_Logement</t>
+  </si>
+  <si>
+    <t>ID_Nationalite</t>
+  </si>
+  <si>
+    <t>ID_StatutEmployeur</t>
+  </si>
+  <si>
+    <t>ID_Position</t>
+  </si>
+  <si>
+    <t>ID_Sexe</t>
+  </si>
+  <si>
+    <t>ID_TypeMenage</t>
+  </si>
+  <si>
+    <t>ID_Employabilite</t>
+  </si>
+  <si>
+    <t>AAC</t>
+  </si>
+  <si>
+    <t>ACTEU6</t>
+  </si>
+  <si>
+    <t>AGE3</t>
+  </si>
+  <si>
+    <t>AIDFAM</t>
+  </si>
+  <si>
+    <t>ANNEE</t>
+  </si>
+  <si>
+    <t>CHPUB</t>
+  </si>
+  <si>
+    <t>INSCONT</t>
+  </si>
+  <si>
+    <t>COURED</t>
+  </si>
+  <si>
+    <t>CREACCP</t>
+  </si>
+  <si>
+    <t>CSA</t>
+  </si>
+  <si>
+    <t>DIP11</t>
+  </si>
+  <si>
+    <t>IDENTM</t>
+  </si>
+  <si>
+    <t>NFRRED</t>
+  </si>
+  <si>
+    <t>PUB3FP</t>
+  </si>
+  <si>
+    <t>QPRC</t>
+  </si>
+  <si>
+    <t>SEXE</t>
+  </si>
+  <si>
+    <t>TYPMEN7</t>
+  </si>
+  <si>
+    <t>Champ source</t>
+  </si>
+  <si>
+    <t>Champ BDD</t>
+  </si>
+  <si>
+    <t>T_ODS_Employabilite</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source  </t>
+  </si>
+  <si>
+    <t>Fichier plat excel</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Fichier plat dbf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom table </t>
+  </si>
+  <si>
+    <t>Referentiel</t>
+  </si>
+  <si>
+    <t>ID_Ref</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Libelle</t>
+  </si>
+  <si>
+    <t>varchar(15)</t>
+  </si>
+  <si>
+    <t>varcahr(250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champ </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -208,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -220,6 +381,8 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +722,7 @@
   <dimension ref="A4:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +739,14 @@
         <v>34</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>31</v>
@@ -758,6 +929,323 @@
       </c>
       <c r="B30" s="5" t="s">
         <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="7" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>